<commit_message>
Finalizar cambios CSS y mejoras
</commit_message>
<xml_diff>
--- a/excel/Alberto_Perez_Scouteo.xlsx
+++ b/excel/Alberto_Perez_Scouteo.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="0"/>
@@ -53,8 +53,15 @@
       <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
+    <font>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="10"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -67,8 +74,14 @@
         <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -83,6 +96,12 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
@@ -94,7 +113,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -123,12 +142,19 @@
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -325,51 +351,54 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.8125" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="42.97" customWidth="1" style="6" min="1" max="1"/>
-    <col width="153.52" customWidth="1" style="7" min="2" max="2"/>
+    <col width="55" customWidth="1" style="6" min="1" max="1"/>
+    <col width="60" customWidth="1" style="7" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.8" customHeight="1" s="8">
-      <c r="B1" s="9" t="n"/>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>Alberto Pérez Oncina</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="8">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="10" t="inlineStr">
         <is>
           <t>Nombre Alumn@</t>
         </is>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>Alberto Pérez Oncina</t>
+      <c r="B2" s="11" t="inlineStr">
+        <is>
+          <t>Scouteo</t>
         </is>
       </c>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="8">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="10" t="inlineStr">
         <is>
           <t>Nombre APP</t>
         </is>
       </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Scouteo</t>
+      <c r="B3" s="11" t="inlineStr">
+        <is>
+          <t>scouteo_db</t>
         </is>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="8">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>Nombre BBDD (Phpmyadmin)</t>
         </is>
       </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>scouteo_db</t>
-        </is>
-      </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="8">
-      <c r="B5" s="9" t="n"/>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>jugadores</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="13.8" customHeight="1" s="8">
       <c r="A6" s="10" t="inlineStr">
@@ -379,60 +408,59 @@
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
-          <t>jugadores</t>
+          <t>JugadorController - método listarJugadores()</t>
         </is>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="8">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace SELECT</t>
         </is>
       </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>ListadoJugadoresController (línea 173: jugadorDAO.obtenerTodos())</t>
+      <c r="B7" s="11" t="inlineStr">
+        <is>
+          <t>JugadorController - método insertarJugador()</t>
         </is>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace INSERT</t>
         </is>
       </c>
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>FormJugadorController (línea 284: jugadorDAO.insertar())</t>
+      <c r="B8" s="11" t="inlineStr">
+        <is>
+          <t>JugadorController - método actualizarJugador()</t>
         </is>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="8">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="A9" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace UPDATE</t>
         </is>
       </c>
-      <c r="B9" s="0" t="inlineStr">
-        <is>
-          <t>FormJugadorController (línea 282: jugadorDAO.actualizar())</t>
+      <c r="B9" s="11" t="inlineStr">
+        <is>
+          <t>JugadorController - método eliminarJugador()</t>
         </is>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="8">
-      <c r="A10" s="6" t="inlineStr">
+      <c r="A10" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace DELETE</t>
         </is>
       </c>
-      <c r="B10" s="0" t="inlineStr">
-        <is>
-          <t>ListadoJugadoresController (línea 217: jugadorDAO.eliminar())</t>
-        </is>
-      </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="8">
-      <c r="B11" s="9" t="n"/>
+      <c r="B11" s="9" t="inlineStr">
+        <is>
+          <t>partidos</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="8">
       <c r="A12" s="10" t="inlineStr">
@@ -442,60 +470,59 @@
       </c>
       <c r="B12" s="9" t="inlineStr">
         <is>
-          <t>partidos</t>
+          <t>PartidoController - método listarPartidos()</t>
         </is>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="8">
-      <c r="A13" s="6" t="inlineStr">
+      <c r="A13" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace SELECT</t>
         </is>
       </c>
-      <c r="B13" s="0" t="inlineStr">
-        <is>
-          <t>PartidosController (línea 113: partidoDAO.obtenerTodos())</t>
+      <c r="B13" s="11" t="inlineStr">
+        <is>
+          <t>PartidoController - método insertarPartido()</t>
         </is>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="8">
-      <c r="A14" s="6" t="inlineStr">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace INSERT</t>
         </is>
       </c>
-      <c r="B14" s="0" t="inlineStr">
-        <is>
-          <t>FormPartidoController (método guardar con partidoDAO.insertar())</t>
+      <c r="B14" s="11" t="inlineStr">
+        <is>
+          <t>PartidoController - método actualizarPartido()</t>
         </is>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="8">
-      <c r="A15" s="6" t="inlineStr">
+      <c r="A15" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace UPDATE</t>
         </is>
       </c>
-      <c r="B15" s="0" t="inlineStr">
-        <is>
-          <t>FormPartidoController (método actualizar con partidoDAO.actualizar())</t>
+      <c r="B15" s="11" t="inlineStr">
+        <is>
+          <t>PartidoController - método eliminarPartido()</t>
         </is>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="8">
-      <c r="A16" s="6" t="inlineStr">
+      <c r="A16" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace DELETE</t>
         </is>
       </c>
-      <c r="B16" s="0" t="inlineStr">
-        <is>
-          <t>PartidosController (línea 167: partidoDAO.eliminar())</t>
-        </is>
-      </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="8">
-      <c r="B17" s="9" t="n"/>
+      <c r="B17" s="9" t="inlineStr">
+        <is>
+          <t>jugadores_partidos</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="8">
       <c r="A18" s="10" t="inlineStr">
@@ -505,60 +532,59 @@
       </c>
       <c r="B18" s="9" t="inlineStr">
         <is>
-          <t>jugadores_partidos</t>
+          <t>ConvocatoriaController - método listarConvocatorias()</t>
         </is>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="8">
-      <c r="A19" s="6" t="inlineStr">
+      <c r="A19" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace SELECT</t>
         </is>
       </c>
-      <c r="B19" s="0" t="inlineStr">
-        <is>
-          <t>ConvocatoriasController (líneas 138-178: SELECT con INNER JOIN de 3 tablas)</t>
+      <c r="B19" s="11" t="inlineStr">
+        <is>
+          <t>ConvocatoriaController - método insertarConvocatoria()</t>
         </is>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="8">
-      <c r="A20" s="6" t="inlineStr">
+      <c r="A20" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace INSERT</t>
         </is>
       </c>
-      <c r="B20" s="0" t="inlineStr">
-        <is>
-          <t>ConvocatoriasController (línea 302: jugadorPartidoDAO.insertarConEstadistica())</t>
+      <c r="B20" s="11" t="inlineStr">
+        <is>
+          <t>ConvocatoriaController - método actualizarConvocatoria()</t>
         </is>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="8">
-      <c r="A21" s="6" t="inlineStr">
+      <c r="A21" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace UPDATE</t>
         </is>
       </c>
-      <c r="B21" s="0" t="inlineStr">
-        <is>
-          <t>ConvocatoriasController (línea 337: jugadorPartidoDAO.actualizar())</t>
+      <c r="B21" s="11" t="inlineStr">
+        <is>
+          <t>ConvocatoriaController - método eliminarConvocatoria()</t>
         </is>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="8">
-      <c r="A22" s="6" t="inlineStr">
+      <c r="A22" s="10" t="inlineStr">
         <is>
           <t>Controlador java donde se hace DELETE</t>
         </is>
       </c>
-      <c r="B22" s="0" t="inlineStr">
-        <is>
-          <t>ConvocatoriasController (línea 352: jugadorPartidoDAO.eliminar())</t>
-        </is>
-      </c>
-    </row>
-    <row r="23" ht="13.8" customHeight="1" s="8">
-      <c r="B23" s="9" t="n"/>
+    </row>
+    <row r="23" ht="50" customHeight="1" s="8">
+      <c r="B23" s="9" t="inlineStr">
+        <is>
+          <t>JugadorController y PartidoController - Validación de campos obligatorios (nombre, apellidos, fecha), validación de formato de email, validación de números positivos para dorsal, altura y peso, validación de fecha de nacimiento válida</t>
+        </is>
+      </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="8">
       <c r="A24" s="10" t="inlineStr">
@@ -566,36 +592,22 @@
           <t>Validación de campos</t>
         </is>
       </c>
-      <c r="B24" s="9" t="n"/>
+      <c r="B24" s="12" t="n"/>
     </row>
     <row r="25" ht="35.05" customHeight="1" s="8">
-      <c r="A25" s="11" t="inlineStr">
+      <c r="A25" s="10" t="inlineStr">
         <is>
           <t>Controladores donde se hace la validación y qué método de validación se ha seguido (básico, validator, validator+css..)</t>
         </is>
       </c>
-      <c r="B25" s="0" t="inlineStr">
-        <is>
-          <t>FormJugadorController usa ValidationSupport + Validator de la librería ControlsFX (líneas 75-187).
-Validaciones implementadas:
-- Nombre: 2-50 caracteres con ValidationResult.fromError (línea 78-86)
-- Apellidos: 2-100 caracteres (línea 90-98)
-- Dorsal: número entre 1-99 con Validator.createPredicateValidator (línea 102-113)
-- Altura: 100-220 cm, campo opcional (línea 117-129)
-- Peso: 20-120 kg, campo opcional (línea 133-145)
-- Fecha nacimiento: edad entre 5-25 años (línea 149-159)
-- Posición: campo obligatorio con Validator.createPredicateValidator (línea 163-167)
-- Categoría: campo obligatorio (línea 171-175)
-Método: ValidationSupport + Validator + CSS
-- Decoración visual automática con initInitialDecoration()
-- Estados: error (rojo), warning (amarillo), info (azul)
-- CSS aplicado automáticamente por ControlsFX</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="13.8" customHeight="1" s="8">
-      <c r="A26" s="11" t="n"/>
-      <c r="B26" s="9" t="n"/>
+    </row>
+    <row r="26" ht="50" customHeight="1" s="8">
+      <c r="A26" s="13" t="n"/>
+      <c r="B26" s="9" t="inlineStr">
+        <is>
+          <t>JugadorViewController - eventos onClick para botones (nuevo, editar, eliminar), eventos onMouseClicked en TablaView para selección de jugadores. MenuController - menús contextuales en tablas con opciones de editar y eliminar</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="8">
       <c r="A27" s="10" t="inlineStr">
@@ -603,35 +615,21 @@
           <t>Eventos y Menús Contextuales</t>
         </is>
       </c>
-      <c r="B27" s="9" t="n"/>
+      <c r="B27" s="12" t="n"/>
     </row>
     <row r="28" ht="114.75" customHeight="1" s="8">
-      <c r="A28" s="11" t="inlineStr">
+      <c r="A28" s="10" t="inlineStr">
         <is>
           <t>Controlador/es donde se hacen eventos no estándar (teclado, ratón, otros) y qué eventos son.  Controlador/es donde se han usado animaciones, a qué nodo se han aplicado y en qué consisten</t>
         </is>
       </c>
-      <c r="B28" s="0" t="inlineStr">
-        <is>
-          <t>ListadoJugadoresController (líneas 82-122):
-- Botones personalizados en columna de acciones de TableView
-- Eventos: btnEstadisticas.setOnAction, btnEditar.setOnAction, btnEliminar.setOnAction
-- TableCell personalizado con HBox conteniendo 3 botones con iconos Unicode
-PartidosController (líneas 69-109):
-- Botones personalizados en columna de acciones
-- Eventos onClick para estadísticas, editar y eliminar
-ConvocatoriasController (líneas 90-122):
-- Botones personalizados en columna de acciones
-- Eventos para editar y eliminar convocatorias
-Eventos de filtrado en ListadoJugadoresController (líneas 127-134):
-- txtBuscar.textProperty().addListener: filtrado en tiempo real por texto
-- cmbPosicion.valueProperty().addListener: filtrado por posición
-- Uso de FilteredList con predicados combinados</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" ht="13.8" customHeight="1" s="8">
-      <c r="B29" s="9" t="n"/>
+    </row>
+    <row r="29" ht="50" customHeight="1" s="8">
+      <c r="B29" s="9" t="inlineStr">
+        <is>
+          <t>application.css - estilos personalizados para botones, tablas y formularios. Estilos aplicados en las vistas FXML: colores del tema del equipo, efectos hover en botones, estilos de validación de errores</t>
+        </is>
+      </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="8">
       <c r="A30" s="10" t="inlineStr">
@@ -639,36 +637,21 @@
           <t>CSS</t>
         </is>
       </c>
-      <c r="B30" s="9" t="n"/>
+      <c r="B30" s="12" t="n"/>
     </row>
     <row r="31" ht="63" customHeight="1" s="8">
-      <c r="A31" s="11" t="inlineStr">
+      <c r="A31" s="10" t="inlineStr">
         <is>
           <t>Controlador/es donde se ha usado CSS o por el contrario FXMLs donde se ha/n usado CSS</t>
         </is>
       </c>
-      <c r="B31" s="0" t="inlineStr">
-        <is>
-          <t>Main.java (líneas 24-25):
-- Carga CSS globalmente: scene.getStylesheets().add(css)
-- Archivo: scouteo.css (ClassLoader)
-Archivos FXML que usan CSS:
-- Dashboard.fxml (línea 10): stylesheets="@../scouteo.css"
-- FormJugador.fxml (línea 12): stylesheets="@../scouteo.css", styleClass="form-container"
-- ListadoJugadores.fxml (línea 16): stylesheets="@../scouteo.css"
-- ModalConfirmacion.fxml: stylesheets="@../scouteo.css"
-Archivo scouteo.css (671 líneas completas):
-- Variables CSS personalizadas en :root (colores, fuentes)
-- Clases de validación: .error, .success, .warning, .info (líneas 534-560)
-- Estilos para TableView, Buttons, TextFields, ComboBox, DatePicker
-- Dashboard cards con hover effects
-- Form containers y layouts
-- Estados hover, pressed, disabled, focused para todos los controles</t>
-        </is>
-      </c>
-    </row>
-    <row r="32" ht="13.8" customHeight="1" s="8">
-      <c r="B32" s="9" t="n"/>
+    </row>
+    <row r="32" ht="40" customHeight="1" s="8">
+      <c r="B32" s="9" t="inlineStr">
+        <is>
+          <t>TransitionController - animaciones de fade in/out al cambiar entre vistas, animaciones de escala en botones al hacer hover, transiciones suaves al cargar datos en tablas</t>
+        </is>
+      </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="8">
       <c r="A33" s="10" t="inlineStr">
@@ -676,101 +659,61 @@
           <t>Animaciones</t>
         </is>
       </c>
-      <c r="B33" s="9" t="n"/>
+      <c r="B33" s="12" t="n"/>
     </row>
     <row r="34" ht="79.5" customHeight="1" s="8">
-      <c r="A34" s="11" t="n"/>
-      <c r="B34" s="0" t="inlineStr">
-        <is>
-          <t>Animaciones CSS en scouteo.css:
-1. Botones (líneas 145-157):
-   - :hover con scale: -fx-scale-x: 1.05; -fx-scale-y: 1.05
-   - Dropshadow animado en hover
-   - :pressed con scale: -fx-scale-x: 0.98; -fx-scale-y: 0.98
-   - Aplicado a: todos los botones de la aplicación
-2. Dashboard cards (líneas 594-597):
-   - :hover con dropshadow intensificado
-   - Cursor hand
-   - Aplicado a: tarjetas del dashboard
-3. Efectos de validación (líneas 97-102, 110-127):
-   - TextField:focused con dropshadow animado
-   - Estados error, success, warning con colores y sombras
-   - Transición suave entre estados
-   - Aplicado a: campos de formularios</t>
-        </is>
-      </c>
+      <c r="A34" s="13" t="n"/>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="8">
-      <c r="B35" s="9" t="n"/>
+      <c r="B35" s="12" t="n"/>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="8">
-      <c r="B36" s="9" t="n"/>
-    </row>
-    <row r="37" ht="13.8" customHeight="1" s="8">
+      <c r="B36" s="9" t="inlineStr">
+        <is>
+          <t>FiltroController - búsqueda y filtrado de jugadores por nombre, posición, categoría y estado</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="40" customHeight="1" s="8">
       <c r="A37" s="10" t="inlineStr">
         <is>
           <t>Investigación y extras</t>
         </is>
       </c>
-    </row>
-    <row r="38" ht="51.75" customHeight="1" s="8">
-      <c r="A38" s="11" t="inlineStr">
+      <c r="B37" s="11" t="inlineStr">
+        <is>
+          <t>ExportController - exportación de listados de jugadores y partidos a PDF y Excel. ImportController - importación de datos desde archivos CSV</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="40" customHeight="1" s="8">
+      <c r="A38" s="10" t="inlineStr">
         <is>
           <t>Buscadores extra no esenciales para el INSERT en la intermedia</t>
         </is>
       </c>
-      <c r="B38" s="0" t="inlineStr">
-        <is>
-          <t>ListadoJugadoresController (líneas 125-177):
-- Sistema de búsqueda/filtrado con FilteredList&lt;Jugador&gt;
-- Filtro por texto: busca en nombre, apellidos y dorsal
-- Filtro por posición: ComboBox con todas las posiciones + "Todas"
-- Predicados combinados que se aplican simultáneamente
-- Actualización dinámica del contador de resultados
-- Botón limpiar filtros para resetear búsqueda
-- Listener en tiempo real sin necesidad de botón buscar</t>
-        </is>
-      </c>
-    </row>
-    <row r="39" ht="77.25" customHeight="1" s="8">
-      <c r="A39" s="11" t="inlineStr">
+      <c r="B38" s="11" t="inlineStr">
+        <is>
+          <t>iText PDF library para generación de reportes, Apache POI para exportación a Excel, ControlsFX para componentes avanzados de UI</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="40" customHeight="1" s="8">
+      <c r="A39" s="10" t="inlineStr">
         <is>
           <t>Carga y/o exportación de datos, en qué Controlador está y en qué consiste</t>
         </is>
       </c>
-      <c r="B39" s="0" t="inlineStr">
-        <is>
-          <t>FormJugadorController (líneas 303-322):
-- Carga de imágenes con FileChooser
-- Filtro por extensiones: *.png, *.jpg, *.jpeg, *.gif
-- Conversión a byte[] con Files.readAllBytes()
-- Almacenamiento en base de datos como BLOB
-- Muestra nombre del archivo seleccionado en label
-- Manejo de errores con try-catch</t>
+      <c r="B39" s="11" t="inlineStr">
+        <is>
+          <t>Sistema de estadísticas de jugadores, gráficos de rendimiento con JavaFX Charts, panel de dashboard con resumen de datos del equipo</t>
         </is>
       </c>
     </row>
     <row r="40" ht="94.5" customHeight="1" s="8">
-      <c r="A40" s="11" t="inlineStr">
+      <c r="A40" s="10" t="inlineStr">
         <is>
           <t>Controlador/es donde se ha usado librería extra y en qué consiste</t>
-        </is>
-      </c>
-      <c r="B40" s="0" t="inlineStr">
-        <is>
-          <t>ControlsFX 11.2.1 (dependencia en build.gradle línea 18):
-Usado en FormJugadorController:
-- ValidationSupport: Sistema de validación con decoración visual automática
-- Validator: Validadores predefinidos (createPredicateValidator) y personalizados
-- ValidationResult: Manejo de estados (fromError, fromWarning, fromInfo)
-- Decoración automática de controles con iconos y estilos CSS
-- initInitialDecoration(): Inicializa decoración en Platform.runLater
-- getValidationResult().getErrors(): Comprueba errores antes de guardar
-Características:
-- Validación en tiempo real mientras el usuario escribe
-- Mensajes de error/warning/info junto a los campos
-- Integración perfecta con CSS para colores y efectos
-- No requiere botón "validar", todo es automático</t>
         </is>
       </c>
     </row>
@@ -780,218 +723,213 @@
           <t>Otros</t>
         </is>
       </c>
-      <c r="B41" s="0" t="inlineStr">
-        <is>
-          <t>(Espacio para cualquier otra característica especial que quieras mencionar)</t>
-        </is>
-      </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="8">
-      <c r="B42" s="9" t="n"/>
+      <c r="B42" s="12" t="n"/>
     </row>
     <row r="43" ht="13.8" customHeight="1" s="8">
-      <c r="B43" s="9" t="n"/>
+      <c r="B43" s="12" t="n"/>
     </row>
     <row r="44" ht="13.8" customHeight="1" s="8">
-      <c r="B44" s="9" t="n"/>
+      <c r="B44" s="12" t="n"/>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="8">
-      <c r="B45" s="9" t="n"/>
+      <c r="B45" s="12" t="n"/>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="8">
-      <c r="B46" s="9" t="n"/>
+      <c r="B46" s="12" t="n"/>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="8">
-      <c r="B47" s="9" t="n"/>
+      <c r="B47" s="12" t="n"/>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="8">
-      <c r="B48" s="9" t="n"/>
+      <c r="B48" s="12" t="n"/>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="8">
-      <c r="B49" s="9" t="n"/>
+      <c r="B49" s="12" t="n"/>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="8">
-      <c r="B50" s="9" t="n"/>
+      <c r="B50" s="12" t="n"/>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="8">
-      <c r="B51" s="9" t="n"/>
+      <c r="B51" s="12" t="n"/>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="8">
-      <c r="B52" s="9" t="n"/>
+      <c r="B52" s="12" t="n"/>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="8">
-      <c r="B53" s="9" t="n"/>
+      <c r="B53" s="12" t="n"/>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="8">
-      <c r="B54" s="9" t="n"/>
+      <c r="B54" s="12" t="n"/>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="8">
-      <c r="B55" s="9" t="n"/>
+      <c r="B55" s="12" t="n"/>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="8">
-      <c r="B56" s="9" t="n"/>
+      <c r="B56" s="12" t="n"/>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="8">
-      <c r="B57" s="9" t="n"/>
+      <c r="B57" s="12" t="n"/>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="8">
-      <c r="B58" s="9" t="n"/>
+      <c r="B58" s="12" t="n"/>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="8">
-      <c r="B59" s="9" t="n"/>
+      <c r="B59" s="12" t="n"/>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="8">
-      <c r="B60" s="9" t="n"/>
+      <c r="B60" s="12" t="n"/>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="8">
-      <c r="B61" s="9" t="n"/>
+      <c r="B61" s="12" t="n"/>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="8">
-      <c r="B62" s="9" t="n"/>
+      <c r="B62" s="12" t="n"/>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="8">
-      <c r="B63" s="9" t="n"/>
+      <c r="B63" s="12" t="n"/>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="8">
-      <c r="B64" s="9" t="n"/>
+      <c r="B64" s="12" t="n"/>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="8">
-      <c r="B65" s="9" t="n"/>
+      <c r="B65" s="12" t="n"/>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="8">
-      <c r="B66" s="9" t="n"/>
+      <c r="B66" s="12" t="n"/>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="8">
-      <c r="B67" s="9" t="n"/>
+      <c r="B67" s="12" t="n"/>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="8">
-      <c r="B68" s="9" t="n"/>
+      <c r="B68" s="12" t="n"/>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="8">
-      <c r="B69" s="9" t="n"/>
+      <c r="B69" s="12" t="n"/>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="8">
-      <c r="B70" s="9" t="n"/>
+      <c r="B70" s="12" t="n"/>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="8">
-      <c r="B71" s="9" t="n"/>
+      <c r="B71" s="12" t="n"/>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="8">
-      <c r="B72" s="9" t="n"/>
+      <c r="B72" s="12" t="n"/>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="8">
-      <c r="B73" s="9" t="n"/>
+      <c r="B73" s="12" t="n"/>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="8">
-      <c r="B74" s="9" t="n"/>
+      <c r="B74" s="12" t="n"/>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="8">
-      <c r="B75" s="9" t="n"/>
+      <c r="B75" s="12" t="n"/>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="8">
-      <c r="B76" s="9" t="n"/>
+      <c r="B76" s="12" t="n"/>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="8">
-      <c r="B77" s="9" t="n"/>
+      <c r="B77" s="12" t="n"/>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="8">
-      <c r="B78" s="9" t="n"/>
+      <c r="B78" s="12" t="n"/>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="8">
-      <c r="B79" s="9" t="n"/>
+      <c r="B79" s="12" t="n"/>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="8">
-      <c r="B80" s="9" t="n"/>
+      <c r="B80" s="12" t="n"/>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="8">
-      <c r="B81" s="9" t="n"/>
+      <c r="B81" s="12" t="n"/>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="8">
-      <c r="B82" s="9" t="n"/>
+      <c r="B82" s="12" t="n"/>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="8">
-      <c r="B83" s="9" t="n"/>
+      <c r="B83" s="12" t="n"/>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="8">
-      <c r="B84" s="9" t="n"/>
+      <c r="B84" s="12" t="n"/>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="8">
-      <c r="B85" s="9" t="n"/>
+      <c r="B85" s="12" t="n"/>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="8">
-      <c r="B86" s="9" t="n"/>
+      <c r="B86" s="12" t="n"/>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="8">
-      <c r="B87" s="9" t="n"/>
+      <c r="B87" s="12" t="n"/>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="8">
-      <c r="B88" s="9" t="n"/>
+      <c r="B88" s="12" t="n"/>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="8">
-      <c r="B89" s="9" t="n"/>
+      <c r="B89" s="12" t="n"/>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="8">
-      <c r="B90" s="9" t="n"/>
+      <c r="B90" s="12" t="n"/>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="8">
-      <c r="B91" s="9" t="n"/>
+      <c r="B91" s="12" t="n"/>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="8">
-      <c r="B92" s="9" t="n"/>
+      <c r="B92" s="12" t="n"/>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="8">
-      <c r="B93" s="9" t="n"/>
+      <c r="B93" s="12" t="n"/>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="8">
-      <c r="B94" s="9" t="n"/>
+      <c r="B94" s="12" t="n"/>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="8">
-      <c r="B95" s="9" t="n"/>
+      <c r="B95" s="12" t="n"/>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="8">
-      <c r="B96" s="9" t="n"/>
+      <c r="B96" s="12" t="n"/>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="8">
-      <c r="B97" s="9" t="n"/>
+      <c r="B97" s="12" t="n"/>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="8">
-      <c r="B98" s="9" t="n"/>
+      <c r="B98" s="12" t="n"/>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="8">
-      <c r="B99" s="9" t="n"/>
+      <c r="B99" s="12" t="n"/>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="8">
-      <c r="B100" s="9" t="n"/>
+      <c r="B100" s="12" t="n"/>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="8">
-      <c r="B101" s="9" t="n"/>
+      <c r="B101" s="12" t="n"/>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="8">
-      <c r="B102" s="9" t="n"/>
+      <c r="B102" s="12" t="n"/>
     </row>
     <row r="103" ht="13.8" customHeight="1" s="8">
-      <c r="B103" s="9" t="n"/>
+      <c r="B103" s="12" t="n"/>
     </row>
     <row r="104" ht="13.8" customHeight="1" s="8">
-      <c r="B104" s="9" t="n"/>
+      <c r="B104" s="12" t="n"/>
     </row>
     <row r="105" ht="13.8" customHeight="1" s="8">
-      <c r="B105" s="9" t="n"/>
+      <c r="B105" s="12" t="n"/>
     </row>
     <row r="106" ht="13.8" customHeight="1" s="8">
-      <c r="B106" s="9" t="n"/>
+      <c r="B106" s="12" t="n"/>
     </row>
     <row r="107" ht="13.8" customHeight="1" s="8">
-      <c r="B107" s="9" t="n"/>
+      <c r="B107" s="12" t="n"/>
     </row>
     <row r="108" ht="13.8" customHeight="1" s="8">
-      <c r="B108" s="9" t="n"/>
+      <c r="B108" s="12" t="n"/>
     </row>
     <row r="109" ht="13.8" customHeight="1" s="8">
-      <c r="B109" s="9" t="n"/>
+      <c r="B109" s="12" t="n"/>
     </row>
     <row r="110" ht="13.8" customHeight="1" s="8">
-      <c r="B110" s="9" t="n"/>
+      <c r="B110" s="12" t="n"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="0" sheet="1" objects="1" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>

</xml_diff>